<commit_message>
Feb 19 - results shown as a list view
</commit_message>
<xml_diff>
--- a/res/raw/featureslist.xlsx
+++ b/res/raw/featureslist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Description</t>
   </si>
@@ -33,33 +33,18 @@
     <t>Bug</t>
   </si>
   <si>
-    <t>To Do</t>
-  </si>
-  <si>
-    <t>Get rid of Toast that comes up when location is found</t>
-  </si>
-  <si>
-    <t>Be more efficient with location listener (right now it keeps pinging for updates too often)</t>
-  </si>
-  <si>
     <t>Put in more locations with their GeoPoints looked up</t>
   </si>
   <si>
     <t>Priority</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
     <t>Medium</t>
   </si>
   <si>
-    <t>Re-factor code into code blocks</t>
-  </si>
-  <si>
     <t>Assigned To</t>
   </si>
   <si>
@@ -76,6 +61,9 @@
   </si>
   <si>
     <t>Build calculations to figure out probability of availability of spots</t>
+  </si>
+  <si>
+    <t>Location listener called when orientation changes</t>
   </si>
 </sst>
 </file>
@@ -459,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -481,10 +469,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -493,16 +481,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -513,24 +501,24 @@
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -538,69 +526,41 @@
         <v>13</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>